<commit_message>
vm test 8 linux vm
</commit_message>
<xml_diff>
--- a/database_data.xlsx
+++ b/database_data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simen\git_stuff\socketing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02E6CD28-662B-4255-B8C8-E916C3F6F672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35318DCF-1806-4839-98C1-AF2DDEB033EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10360" xr2:uid="{F5EABCD3-48A0-4E42-B4EB-77BAFB836925}"/>
+    <workbookView xWindow="19090" yWindow="4800" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{F5EABCD3-48A0-4E42-B4EB-77BAFB836925}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Teknisk dokumentasjon" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>player_name</t>
   </si>
@@ -81,6 +82,45 @@
   </si>
   <si>
     <t>skin</t>
+  </si>
+  <si>
+    <t>ubuntu_server</t>
+  </si>
+  <si>
+    <t>Vm</t>
+  </si>
+  <si>
+    <t>name:</t>
+  </si>
+  <si>
+    <t>simen</t>
+  </si>
+  <si>
+    <t>servername:</t>
+  </si>
+  <si>
+    <t>simens_server_ubuntu</t>
+  </si>
+  <si>
+    <t>username:</t>
+  </si>
+  <si>
+    <t>password:</t>
+  </si>
+  <si>
+    <t>simen123</t>
+  </si>
+  <si>
+    <t>mysql password:</t>
+  </si>
+  <si>
+    <t>root</t>
+  </si>
+  <si>
+    <t>simenerkul</t>
+  </si>
+  <si>
+    <t>mysql user:</t>
   </si>
 </sst>
 </file>
@@ -233,13 +273,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -563,7 +602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF4F1E67-076D-4246-A6DC-EC7109C6B408}">
   <dimension ref="F7:Q12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
@@ -596,7 +635,7 @@
       <c r="N7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="Q7" s="10" t="s">
+      <c r="Q7" s="9" t="s">
         <v>14</v>
       </c>
     </row>
@@ -604,81 +643,148 @@
       <c r="F8" s="4">
         <v>1</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" t="s">
         <v>2</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="5" t="s">
         <v>5</v>
       </c>
       <c r="K8" s="4"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="6"/>
-      <c r="Q8" s="11"/>
+      <c r="N8" s="5"/>
+      <c r="Q8" s="10"/>
     </row>
     <row r="9" spans="6:17" x14ac:dyDescent="0.25">
       <c r="F9" s="4">
         <v>2</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" t="s">
         <v>3</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="5" t="s">
         <v>6</v>
       </c>
       <c r="K9" s="4"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="6"/>
-      <c r="Q9" s="11"/>
+      <c r="N9" s="5"/>
+      <c r="Q9" s="10"/>
     </row>
     <row r="10" spans="6:17" x14ac:dyDescent="0.25">
       <c r="F10" s="4">
         <v>3</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" t="s">
         <v>2</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="5" t="s">
         <v>7</v>
       </c>
       <c r="K10" s="4"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="6"/>
-      <c r="Q10" s="11"/>
+      <c r="N10" s="5"/>
+      <c r="Q10" s="10"/>
     </row>
     <row r="11" spans="6:17" x14ac:dyDescent="0.25">
       <c r="F11" s="4">
         <v>4</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G11" t="s">
         <v>3</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="5" t="s">
         <v>8</v>
       </c>
       <c r="K11" s="4"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="6"/>
-      <c r="Q11" s="11"/>
+      <c r="N11" s="5"/>
+      <c r="Q11" s="10"/>
     </row>
     <row r="12" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F12" s="7">
+      <c r="F12" s="6">
         <v>5</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G12" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="H12" s="9" t="s">
+      <c r="H12" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="K12" s="7"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="9"/>
-      <c r="Q12" s="12"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="8"/>
+      <c r="Q12" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DBD91FE-0422-43E5-965D-91CB584B29FD}">
+  <dimension ref="C4:E12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
vm test noe sånt
</commit_message>
<xml_diff>
--- a/database_data.xlsx
+++ b/database_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simen\git_stuff\socketing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35318DCF-1806-4839-98C1-AF2DDEB033EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA60C2C9-4310-42BB-B5F3-BC659C2840E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="4800" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{F5EABCD3-48A0-4E42-B4EB-77BAFB836925}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F5EABCD3-48A0-4E42-B4EB-77BAFB836925}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>